<commit_message>
Updated output job and assembly drawings
</commit_message>
<xml_diff>
--- a/pira-smart-PCB/Project Outputs for pira-smart-PCB/BOM/Bill of Materials production-pira-smart-PCB.xlsx
+++ b/pira-smart-PCB/Project Outputs for pira-smart-PCB/BOM/Bill of Materials production-pira-smart-PCB.xlsx
@@ -3,11 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Goran\Documents\Repositories\pira-smart-hardware\pira-smart-PCB\Project Outputs for pira-smart-PCB\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2610" yWindow="105" windowWidth="18990" windowHeight="11760"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="255">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -115,10 +110,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>3/28/2018</t>
-  </si>
-  <si>
-    <t>12:31:00 PM</t>
+    <t>4/4/2018</t>
+  </si>
+  <si>
+    <t>12:13:49 PM</t>
   </si>
   <si>
     <t>PiRa-Smart</t>
@@ -133,9 +128,15 @@
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
+    <t>SE30AFG-M3/6A</t>
+  </si>
+  <si>
     <t>RS1JE361T</t>
   </si>
   <si>
+    <t>RCA060310R0FKEA</t>
+  </si>
+  <si>
     <t>BQ24296RGET</t>
   </si>
   <si>
@@ -145,21 +146,66 @@
     <t>TPS62740DSSR</t>
   </si>
   <si>
+    <t>109990166</t>
+  </si>
+  <si>
+    <t>MMBT3904</t>
+  </si>
+  <si>
+    <t>2N7002,215</t>
+  </si>
+  <si>
     <t>FDSD0420-H-1R5M=P3</t>
   </si>
   <si>
     <t>GRM188R61C475KAAJD</t>
   </si>
   <si>
+    <t>MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, CGA4J1X5R1C106K125AC, CGA4J1X5R1C106K125AC</t>
+  </si>
+  <si>
     <t>MCWR06X2493FTL</t>
   </si>
   <si>
+    <t>MCWR06X1000FTL</t>
+  </si>
+  <si>
     <t>MC0603B473K500CT</t>
   </si>
   <si>
     <t>MC0805X226M6R3CT</t>
   </si>
   <si>
+    <t>MCMR06X103JTL</t>
+  </si>
+  <si>
+    <t>MCMR06X104JTL</t>
+  </si>
+  <si>
+    <t>MCMR06X4701FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X471JTL</t>
+  </si>
+  <si>
+    <t>MCMR06X5601FTL</t>
+  </si>
+  <si>
+    <t>MCWR06X1503FTL</t>
+  </si>
+  <si>
+    <t>MCWR06X2200FTL</t>
+  </si>
+  <si>
+    <t>MCWR06X3302FTL</t>
+  </si>
+  <si>
+    <t>MCWR06X3901FTL</t>
+  </si>
+  <si>
+    <t>Loading...</t>
+  </si>
+  <si>
     <t>MINISMDC150F/24-2</t>
   </si>
   <si>
@@ -181,6 +227,15 @@
     <t>DMG6602SVT</t>
   </si>
   <si>
+    <t>HSMS-C190</t>
+  </si>
+  <si>
+    <t>CR0603-J/-000ELF</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>Manufacturer 1</t>
   </si>
   <si>
@@ -190,15 +245,27 @@
     <t>Vishay Intertechnology</t>
   </si>
   <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
+    <t>Seeed Studio</t>
+  </si>
+  <si>
+    <t>ON Semiconductor / Fairchild</t>
+  </si>
+  <si>
     <t>Nexperia</t>
   </si>
   <si>
     <t>Murata</t>
   </si>
   <si>
+    <t>Multicomp, Multicomp, Multicomp, Multicomp, Multicomp, TDK, TDK</t>
+  </si>
+  <si>
     <t>Multicomp</t>
   </si>
   <si>
@@ -223,12 +290,24 @@
     <t>Diodes</t>
   </si>
   <si>
+    <t>Broadcom Avago</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
+    <t>VISHAY - SE30AFG-M3/6A - RECTIFIER, ESD, 400V, 3A, DO-221AC</t>
+  </si>
+  <si>
     <t>VISHAY - RS1J-E3/61T.. - DIODE, FAST, 1A, 600V, SMD</t>
   </si>
   <si>
+    <t>VISHAY - RCA060310R0FKEA - RES, AUTO, THICK FILM, 10R, 1%, 0603</t>
+  </si>
+  <si>
     <t>IC LI+ CHARGER PWR MGMT 24VQFN</t>
   </si>
   <si>
@@ -238,21 +317,69 @@
     <t>Voltage Regulators - Switching Regulators 360-nA Iq SD Cnvtr w/ Intg Load Switch</t>
   </si>
   <si>
+    <t>RFM95 ULTRA-LONG RANGE TRANSCEIV</t>
+  </si>
+  <si>
+    <t>ON SEMICONDUCTOR/FAIRCHILD - MMBT3904 - TRANSISTOR, NPN, SOT-23</t>
+  </si>
+  <si>
+    <t>NEXPERIA - 2N7002,215 - MOSFET,N CH, 60V,0.3A,SOT23</t>
+  </si>
+  <si>
     <t>MURATA - FDSD0420-H-1R5M=P3 - INDUCTOR, SHIELDED, 1.5UH, 5.1A, 20%</t>
   </si>
   <si>
     <t>MURATA - GRM188R61C475KAAJD - CAP, MLCC, X5R, 4.7UF, 16V, 0603</t>
   </si>
   <si>
+    <t>TDK - CGA4J1X5R1C106K125AC - CAP, MLCC, X5R, 10UF, 16V, 0805</t>
+  </si>
+  <si>
     <t>MULTICOMP         MCWR06X2493FTL             SMD Chip Resistor, Thick Film, 249 kohm, 50 V, 0603 [1608 Metric], 100 mW,  1%, MCWR Series</t>
   </si>
   <si>
+    <t>MULTICOMP - MC0063W06031100R - RES, THICK FILM, 100R, 1%, 0.063W, 0603</t>
+  </si>
+  <si>
     <t>MULTICOMP - MC0603B473K500CT - CAP, MLCC, X7R, 47NF, 50V, 0603</t>
   </si>
   <si>
     <t>MULTICOMP - MC0805X226M6R3CT - CAP, MLCC, X5R, 22UF, 0805</t>
   </si>
   <si>
+    <t>MULTICOMP - MCMR06X103 JTL - RES, CERAMIC, 10K, 5%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCMR06X104 JTL - RES, CERAMIC, 100K, 5%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCMR06X4701FTL - RES, CERAMIC, 4K7, 1%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCMR06X471 JTL - RES, CERAMIC, 470R, 5%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCMR06X5601FTL - RES, CERAMIC, 5K6, 1%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCWR06X1503FTL - RES, THICK FILM, 150KOHM, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCWR06X2200FTL - RES, THICK FILM, 220R, 1%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCWR06X3302FTL - RES, THICK FILM, 33K, 1%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MULTICOMP - MCWR06X3901FTL - RES, THICK FILM, 3K9, 1%, 0.1W, 0603</t>
+  </si>
+  <si>
+    <t>MURATA - GRM188R71C104KA01J - CAP, MLCC, X7R, 0.1UF, 16V, 0603</t>
+  </si>
+  <si>
+    <t>ON SEMICONDUCTOR - MM3Z3V0T1G - ZENER DIODE, 200MW, 3V, SOD-323</t>
+  </si>
+  <si>
     <t>LITTELFUSE - MINISMDC150F/24-2 - POLYSWITCH, SMD, 1812, 1.5A</t>
   </si>
   <si>
@@ -274,9 +401,24 @@
     <t>DIODES INC. - DMG6602SVT - MOSFET, NP CH, , 30V, 3.4, ATSOT23</t>
   </si>
   <si>
+    <t>BROADCOM LIMITED - HSMS-C190 - LED, RED, 10MCD, 626NM</t>
+  </si>
+  <si>
+    <t>BOURNS - CR0603-J/-000ELF - RES, THICK FILM, 0R, 5%, 0.1W, 0603</t>
+  </si>
+  <si>
     <t>Fixed Inductors PFL2015 Shld Power 2.2 uH 20 % 1 A</t>
   </si>
   <si>
+    <t>Header, 4-Pin</t>
+  </si>
+  <si>
+    <t>Jumper</t>
+  </si>
+  <si>
+    <t>MDBT40</t>
+  </si>
+  <si>
     <t>Footprint</t>
   </si>
   <si>
@@ -298,6 +440,9 @@
     <t>SON50P200X265_HS-13N</t>
   </si>
   <si>
+    <t>Lora_module1</t>
+  </si>
+  <si>
     <t>SOT23127P600-8N</t>
   </si>
   <si>
@@ -331,9 +476,21 @@
     <t>TSOT26</t>
   </si>
   <si>
+    <t>LED0603</t>
+  </si>
+  <si>
     <t>INDC2214X15N</t>
   </si>
   <si>
+    <t>HDR1X4</t>
+  </si>
+  <si>
+    <t>JUMPER_NC</t>
+  </si>
+  <si>
+    <t>PCB_MDBT40_10X18</t>
+  </si>
+  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -343,6 +500,9 @@
     <t>D1</t>
   </si>
   <si>
+    <t>R12</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
@@ -352,6 +512,12 @@
     <t>U3</t>
   </si>
   <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
     <t>T6</t>
   </si>
   <si>
@@ -361,21 +527,54 @@
     <t>C2</t>
   </si>
   <si>
+    <t>C1, C4, C5, C6, C11, C13, C14</t>
+  </si>
+  <si>
     <t>R32</t>
   </si>
   <si>
+    <t>R18, R19, R30</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
     <t>C7, C8, C9, C10</t>
   </si>
   <si>
+    <t>R6, R9, R10, R15, R21, R22, R23</t>
+  </si>
+  <si>
+    <t>R16, R17, R20, R31, R33</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
+  </si>
+  <si>
+    <t>R1, R14, R28, R29</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
     <t>D6</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -397,9 +596,24 @@
     <t>T2</t>
   </si>
   <si>
+    <t>D2, D7, D8</t>
+  </si>
+  <si>
+    <t>R2, R4, R11, R26, R27, R34</t>
+  </si>
+  <si>
     <t>L3</t>
   </si>
   <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -409,12 +623,21 @@
     <t>Farnell</t>
   </si>
   <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
     <t>Supplier Part Number 1</t>
   </si>
   <si>
+    <t>2313878</t>
+  </si>
+  <si>
     <t>9550143</t>
   </si>
   <si>
+    <t>2616585</t>
+  </si>
+  <si>
     <t>2373541</t>
   </si>
   <si>
@@ -424,6 +647,12 @@
     <t>2781752</t>
   </si>
   <si>
+    <t>1597-1488-ND</t>
+  </si>
+  <si>
+    <t>9846727</t>
+  </si>
+  <si>
     <t>1510761</t>
   </si>
   <si>
@@ -433,15 +662,54 @@
     <t>2611924</t>
   </si>
   <si>
+    <t>2320856, 2320856, 2320856, 2320856, 2320856, 2210948RL, 2210948RL</t>
+  </si>
+  <si>
     <t>2447306</t>
   </si>
   <si>
+    <t>2447227</t>
+  </si>
+  <si>
     <t>1759116</t>
   </si>
   <si>
     <t>1759415</t>
   </si>
   <si>
+    <t>2073356</t>
+  </si>
+  <si>
+    <t>2073357</t>
+  </si>
+  <si>
+    <t>2073509</t>
+  </si>
+  <si>
+    <t>2073513</t>
+  </si>
+  <si>
+    <t>2073537</t>
+  </si>
+  <si>
+    <t>2447254</t>
+  </si>
+  <si>
+    <t>2447298</t>
+  </si>
+  <si>
+    <t>2447342</t>
+  </si>
+  <si>
+    <t>2447363</t>
+  </si>
+  <si>
+    <t>2688519</t>
+  </si>
+  <si>
+    <t>2463510</t>
+  </si>
+  <si>
     <t>1345929</t>
   </si>
   <si>
@@ -463,6 +731,12 @@
     <t>2061522</t>
   </si>
   <si>
+    <t>2497356</t>
+  </si>
+  <si>
+    <t>2008343</t>
+  </si>
+  <si>
     <t>Supplier Order Qty 1</t>
   </si>
   <si>
@@ -478,6 +752,9 @@
     <t>Supplier Currency 1</t>
   </si>
   <si>
+    <t>GBP</t>
+  </si>
+  <si>
     <t>EUR</t>
   </si>
   <si>
@@ -490,7 +767,7 @@
     <t>75</t>
   </si>
   <si>
-    <t>3/28/2018 12:31:00 PM</t>
+    <t>4/4/2018 12:13:49 PM</t>
   </si>
   <si>
     <t>Bill of Materials production</t>
@@ -503,51 +780,6 @@
   </si>
   <si>
     <t>Bill of Materials</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Coilcraft</t>
-  </si>
-  <si>
-    <t>PFL2015-222MEB</t>
-  </si>
-  <si>
-    <t>SE30AFD-M3/6A</t>
-  </si>
-  <si>
-    <t>SE30AFD-M3/6A -  Standard Recovery Diode, 200 V, 3 A, Single, 980 mV, 40 A</t>
-  </si>
-  <si>
-    <t>2313877</t>
-  </si>
-  <si>
-    <t>2N7002BK</t>
-  </si>
-  <si>
-    <t>NEXPERIA - 2N7002BK - MOSFET Transistor, N Channel, 350 mA, 60 V, 1 ohm, 10 V, 1.6 V</t>
-  </si>
-  <si>
-    <t>NEXPERIA</t>
-  </si>
-  <si>
-    <t>TDZ3V0J</t>
-  </si>
-  <si>
-    <t>NEXPERIA - TDZ3V0J -  Zener Single Diode, 3 V, 500 mW, SOD-323F, 2 %, 2 Pins, 150 °C</t>
-  </si>
-  <si>
-    <t>BSR17A</t>
-  </si>
-  <si>
-    <t>ON SEMICONDUCTOR</t>
-  </si>
-  <si>
-    <t>ON SEMICONDUCTOR - BSR17A -  Bipolar (BJT) Single Transistor, NPN, 40 V, 300 MHz, 350 mW, 200 mA, 100 hFE</t>
-  </si>
-  <si>
-    <t>9846697</t>
   </si>
 </sst>
 </file>
@@ -558,7 +790,7 @@
     <numFmt numFmtId="164" formatCode="[$-C09]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -695,14 +927,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,24 +965,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1222,7 +1430,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1446,6 +1654,19 @@
     <xf numFmtId="2" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1518,43 +1739,251 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="78">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1932,10 +2361,6 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
-    <mruColors>
-      <color rgb="FFCCFFFF"/>
-      <color rgb="FF99CCFF"/>
-    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2287,10 +2712,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2301,7 +2726,7 @@
     <col min="4" max="4" width="28.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="35.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="74" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
@@ -2310,11 +2735,10 @@
     <col min="13" max="13" width="8.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="8" style="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -2331,7 +2755,7 @@
       <c r="N1" s="50"/>
       <c r="O1" s="60"/>
     </row>
-    <row r="2" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="s">
@@ -2339,7 +2763,7 @@
       </c>
       <c r="D2" s="53"/>
       <c r="E2" s="24"/>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="86" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="12"/>
@@ -2352,13 +2776,13 @@
       <c r="N2" s="12"/>
       <c r="O2" s="61"/>
     </row>
-    <row r="3" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="52"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="82" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="13"/>
@@ -2375,13 +2799,13 @@
       <c r="N3" s="36"/>
       <c r="O3" s="62"/>
     </row>
-    <row r="4" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="52"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="83" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="16"/>
@@ -2396,13 +2820,13 @@
       <c r="N4" s="36"/>
       <c r="O4" s="62"/>
     </row>
-    <row r="5" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="84" t="s">
         <v>30</v>
       </c>
       <c r="E5" s="18"/>
@@ -2419,7 +2843,7 @@
       <c r="N5" s="36"/>
       <c r="O5" s="62"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="52"/>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2436,16 +2860,16 @@
       <c r="N6" s="36"/>
       <c r="O6" s="62"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="52"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="85" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="36"/>
@@ -2461,7 +2885,7 @@
       <c r="N7" s="36"/>
       <c r="O7" s="62"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
@@ -2469,11 +2893,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>43187</v>
+        <v>43194</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>43187.662734606478</v>
+        <v>43194.50973946759</v>
       </c>
       <c r="F8" s="36"/>
       <c r="G8" s="20"/>
@@ -2486,1497 +2910,2481 @@
       <c r="N8" s="36"/>
       <c r="O8" s="62"/>
     </row>
-    <row r="9" spans="1:16" s="35" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="35" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
       <c r="B9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="86" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="I9" s="86" t="s">
-        <v>127</v>
-      </c>
-      <c r="J9" s="86" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="94" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="95" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="96" t="s">
-        <v>149</v>
-      </c>
-      <c r="N9" s="96" t="s">
-        <v>150</v>
-      </c>
-      <c r="O9" s="96" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="90" t="s">
+        <v>134</v>
+      </c>
+      <c r="G9" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="90" t="s">
+        <v>199</v>
+      </c>
+      <c r="I9" s="90" t="s">
+        <v>200</v>
+      </c>
+      <c r="J9" s="90" t="s">
+        <v>203</v>
+      </c>
+      <c r="K9" s="98" t="s">
+        <v>240</v>
+      </c>
+      <c r="L9" s="99" t="s">
+        <v>241</v>
+      </c>
+      <c r="M9" s="100" t="s">
+        <v>242</v>
+      </c>
+      <c r="N9" s="100" t="s">
+        <v>243</v>
+      </c>
+      <c r="O9" s="100" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="28">
-        <f t="shared" ref="B10:B30" si="0">ROW(B10) - ROW($B$9)</f>
+        <f>ROW(B10) - ROW($B$9)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="107" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="90" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="90" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="90" t="s">
-        <v>105</v>
+      <c r="C10" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="94" t="s">
+        <v>135</v>
+      </c>
+      <c r="G10" s="94" t="s">
+        <v>159</v>
       </c>
       <c r="H10" s="29">
         <v>2</v>
       </c>
-      <c r="I10" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="107" t="s">
-        <v>166</v>
+      <c r="I10" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J10" s="97" t="s">
+        <v>204</v>
       </c>
       <c r="K10" s="37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L10" s="37">
-        <v>7527</v>
+        <v>557</v>
       </c>
       <c r="M10" s="76">
-        <v>0.32</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="N10" s="76">
-        <f>K10*M10</f>
-        <v>3.2</v>
-      </c>
-      <c r="O10" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P10" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="O10" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B11) - ROW($B$9)</f>
         <v>2</v>
       </c>
-      <c r="C11" s="89" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="89" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="88" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="88" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" s="88" t="s">
-        <v>106</v>
+      <c r="C11" s="93" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="93" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="92" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="92" t="s">
+        <v>160</v>
       </c>
       <c r="H11" s="31">
         <v>1</v>
       </c>
-      <c r="I11" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J11" s="89" t="s">
-        <v>130</v>
+      <c r="I11" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11" s="93" t="s">
+        <v>205</v>
       </c>
       <c r="K11" s="38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L11" s="38">
         <v>5074</v>
       </c>
       <c r="M11" s="77">
-        <v>0.23499999999999999</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="N11" s="77">
-        <f>K11*M11</f>
-        <v>0.94</v>
-      </c>
-      <c r="O11" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P11" s="106" t="s">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="O11" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="52"/>
+      <c r="B12" s="28">
+        <f>ROW(B12) - ROW($B$9)</f>
+        <v>3</v>
+      </c>
+      <c r="C12" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="91" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="94" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="30">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C12" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="88" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="88" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="31">
+      <c r="H12" s="29">
         <v>1</v>
       </c>
-      <c r="I12" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J12" s="89" t="s">
-        <v>131</v>
-      </c>
-      <c r="K12" s="38">
+      <c r="I12" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J12" s="97" t="s">
+        <v>206</v>
+      </c>
+      <c r="K12" s="37">
+        <v>10</v>
+      </c>
+      <c r="L12" s="37">
+        <v>326</v>
+      </c>
+      <c r="M12" s="76">
+        <v>9.1700000000000004E-2</v>
+      </c>
+      <c r="N12" s="76">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="O12" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="30">
+        <f>ROW(B13) - ROW($B$9)</f>
         <v>4</v>
       </c>
-      <c r="L12" s="38">
+      <c r="C13" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="92" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="92" t="s">
+        <v>162</v>
+      </c>
+      <c r="H13" s="31">
+        <v>1</v>
+      </c>
+      <c r="I13" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J13" s="93" t="s">
+        <v>207</v>
+      </c>
+      <c r="K13" s="38">
+        <v>4</v>
+      </c>
+      <c r="L13" s="38">
         <v>251</v>
       </c>
-      <c r="M12" s="77">
+      <c r="M13" s="77">
         <v>2.36</v>
       </c>
-      <c r="N12" s="77">
+      <c r="N13" s="77">
         <v>9.44</v>
       </c>
-      <c r="O12" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P12" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="28">
-        <f t="shared" si="0"/>
+      <c r="O13" s="102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="28">
+        <f>ROW(B14) - ROW($B$9)</f>
+        <v>5</v>
+      </c>
+      <c r="C14" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="91" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="94" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="29">
+        <v>1</v>
+      </c>
+      <c r="I14" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J14" s="97" t="s">
+        <v>208</v>
+      </c>
+      <c r="K14" s="37">
         <v>4</v>
       </c>
-      <c r="C13" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="87" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="90" t="s">
-        <v>108</v>
-      </c>
-      <c r="H13" s="29">
-        <v>1</v>
-      </c>
-      <c r="I13" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J13" s="93" t="s">
-        <v>132</v>
-      </c>
-      <c r="K13" s="37">
-        <v>4</v>
-      </c>
-      <c r="L13" s="37">
-        <v>20</v>
-      </c>
-      <c r="M13" s="76">
+      <c r="L14" s="37">
+        <v>170</v>
+      </c>
+      <c r="M14" s="76">
         <v>2.58</v>
       </c>
-      <c r="N13" s="76">
+      <c r="N14" s="76">
         <v>10.32</v>
       </c>
-      <c r="O13" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P13" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
-      <c r="B14" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="89" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="G14" s="88" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="31">
-        <v>1</v>
-      </c>
-      <c r="I14" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J14" s="89" t="s">
-        <v>133</v>
-      </c>
-      <c r="K14" s="38">
-        <v>4</v>
-      </c>
-      <c r="L14" s="38">
-        <v>2362</v>
-      </c>
-      <c r="M14" s="77">
-        <v>1.44</v>
-      </c>
-      <c r="N14" s="77">
-        <f>K14*M14</f>
-        <v>5.76</v>
-      </c>
-      <c r="O14" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P14" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O14" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B15) - ROW($B$9)</f>
         <v>6</v>
       </c>
-      <c r="C15" s="112" t="s">
-        <v>167</v>
-      </c>
-      <c r="D15" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="88" t="s">
-        <v>168</v>
-      </c>
-      <c r="F15" s="88" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="88" t="s">
-        <v>110</v>
+      <c r="C15" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="92" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="92" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="92" t="s">
+        <v>164</v>
       </c>
       <c r="H15" s="31">
         <v>1</v>
       </c>
-      <c r="I15" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J15" s="113" t="s">
-        <v>134</v>
+      <c r="I15" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J15" s="93" t="s">
+        <v>209</v>
       </c>
       <c r="K15" s="38">
         <v>5</v>
       </c>
       <c r="L15" s="38">
-        <v>405</v>
+        <v>2312</v>
       </c>
       <c r="M15" s="77">
-        <v>0.41399999999999998</v>
+        <v>1.44</v>
       </c>
       <c r="N15" s="77">
-        <f>K15*M15</f>
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="O15" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P15" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7.2</v>
+      </c>
+      <c r="O15" s="102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B16) - ROW($B$9)</f>
         <v>7</v>
       </c>
-      <c r="C16" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="90" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="90" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" s="90" t="s">
-        <v>111</v>
+      <c r="C16" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" s="94" t="s">
+        <v>165</v>
       </c>
       <c r="H16" s="29">
-        <v>2</v>
-      </c>
-      <c r="I16" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J16" s="93" t="s">
-        <v>135</v>
-      </c>
-      <c r="K16" s="37">
-        <v>8</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I16" s="95" t="s">
+        <v>202</v>
+      </c>
+      <c r="J16" s="97" t="s">
+        <v>210</v>
+      </c>
+      <c r="K16" s="37"/>
       <c r="L16" s="37">
-        <v>1228</v>
-      </c>
-      <c r="M16" s="76">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="N16" s="76">
-        <f>K16*M16</f>
-        <v>7.0960000000000001</v>
-      </c>
-      <c r="O16" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P16" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="76"/>
+      <c r="N16" s="76"/>
+      <c r="O16" s="101" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
       <c r="B17" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B17) - ROW($B$9)</f>
         <v>8</v>
       </c>
-      <c r="C17" s="89" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="88" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="88" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="88" t="s">
-        <v>112</v>
+      <c r="C17" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="93" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="92" t="s">
+        <v>142</v>
+      </c>
+      <c r="G17" s="92" t="s">
+        <v>166</v>
       </c>
       <c r="H17" s="31">
         <v>1</v>
       </c>
-      <c r="I17" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J17" s="89" t="s">
-        <v>136</v>
+      <c r="I17" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J17" s="93" t="s">
+        <v>211</v>
       </c>
       <c r="K17" s="38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L17" s="38">
-        <v>1860</v>
+        <v>0</v>
       </c>
       <c r="M17" s="77">
-        <v>0.28000000000000003</v>
+        <v>0.153</v>
       </c>
       <c r="N17" s="77">
-        <f>K17*M17</f>
-        <v>2.8000000000000003</v>
-      </c>
-      <c r="O17" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P17" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="O17" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
-      <c r="B18" s="30">
-        <f t="shared" si="0"/>
+      <c r="B18" s="28">
+        <f>ROW(B18) - ROW($B$9)</f>
         <v>9</v>
       </c>
-      <c r="C18" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="89" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="88" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="88" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="31">
+      <c r="C18" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="94" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="94" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="29">
         <v>1</v>
       </c>
-      <c r="I18" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J18" s="89" t="s">
-        <v>137</v>
-      </c>
-      <c r="K18" s="38">
-        <v>10</v>
-      </c>
-      <c r="L18" s="38">
-        <v>4967</v>
-      </c>
-      <c r="M18" s="77">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="N18" s="77">
-        <f>K18*M18</f>
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="O18" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P18" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J18" s="97" t="s">
+        <v>212</v>
+      </c>
+      <c r="K18" s="37">
+        <v>5</v>
+      </c>
+      <c r="L18" s="37">
+        <v>0</v>
+      </c>
+      <c r="M18" s="76">
+        <v>6.6299999999999998E-2</v>
+      </c>
+      <c r="N18" s="76">
+        <v>0.33150000000000002</v>
+      </c>
+      <c r="O18" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
       <c r="B19" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B19) - ROW($B$9)</f>
         <v>10</v>
       </c>
-      <c r="C19" s="89" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="89" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="88" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="88" t="s">
-        <v>94</v>
-      </c>
-      <c r="G19" s="88" t="s">
-        <v>114</v>
+      <c r="C19" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="93" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="92" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="92" t="s">
+        <v>168</v>
       </c>
       <c r="H19" s="31">
-        <v>1</v>
-      </c>
-      <c r="I19" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J19" s="89" t="s">
-        <v>138</v>
+        <v>2</v>
+      </c>
+      <c r="I19" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J19" s="93" t="s">
+        <v>213</v>
       </c>
       <c r="K19" s="38">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L19" s="38">
-        <v>17398</v>
+        <v>1228</v>
       </c>
       <c r="M19" s="77">
-        <v>1.83E-2</v>
+        <v>0.88700000000000001</v>
       </c>
       <c r="N19" s="77">
-        <f>K19*M19</f>
-        <v>0.183</v>
-      </c>
-      <c r="O19" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P19" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7.0960000000000001</v>
+      </c>
+      <c r="O19" s="102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B20) - ROW($B$9)</f>
         <v>11</v>
       </c>
-      <c r="C20" s="87" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="87" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="90" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="90" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" s="90" t="s">
-        <v>115</v>
+      <c r="C20" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="94" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" s="94" t="s">
+        <v>169</v>
       </c>
       <c r="H20" s="29">
-        <v>4</v>
-      </c>
-      <c r="I20" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J20" s="93" t="s">
-        <v>139</v>
+        <v>1</v>
+      </c>
+      <c r="I20" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J20" s="97" t="s">
+        <v>214</v>
       </c>
       <c r="K20" s="37">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L20" s="37">
-        <v>7375</v>
+        <v>210</v>
       </c>
       <c r="M20" s="76">
-        <v>0.29099999999999998</v>
+        <v>0.248</v>
       </c>
       <c r="N20" s="76">
-        <f>K20*M20</f>
-        <v>4.6559999999999997</v>
-      </c>
-      <c r="O20" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P20" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2.48</v>
+      </c>
+      <c r="O20" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B21) - ROW($B$9)</f>
         <v>12</v>
       </c>
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="93" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="92" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="89" t="s">
-        <v>169</v>
-      </c>
-      <c r="E21" s="88" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" s="88" t="s">
-        <v>96</v>
-      </c>
-      <c r="G21" s="88" t="s">
-        <v>116</v>
-      </c>
       <c r="H21" s="31">
-        <v>1</v>
-      </c>
-      <c r="I21" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J21" s="114">
-        <v>2069510</v>
-      </c>
-      <c r="K21" s="38">
-        <v>5</v>
-      </c>
-      <c r="L21" s="38">
-        <v>1270</v>
-      </c>
-      <c r="M21" s="77">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="N21" s="77">
-        <f>K21*M21</f>
-        <v>1.135</v>
-      </c>
-      <c r="O21" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P21" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J21" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="77"/>
+      <c r="N21" s="77"/>
+      <c r="O21" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B22) - ROW($B$9)</f>
         <v>13</v>
       </c>
-      <c r="C22" s="87" t="s">
-        <v>172</v>
-      </c>
-      <c r="D22" s="87" t="s">
-        <v>173</v>
-      </c>
-      <c r="E22" s="90" t="s">
-        <v>174</v>
-      </c>
-      <c r="F22" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="90" t="s">
-        <v>117</v>
+      <c r="C22" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="F22" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="94" t="s">
+        <v>171</v>
       </c>
       <c r="H22" s="29">
         <v>1</v>
       </c>
-      <c r="I22" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J22" s="111" t="s">
-        <v>175</v>
+      <c r="I22" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J22" s="97" t="s">
+        <v>216</v>
       </c>
       <c r="K22" s="37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L22" s="37">
-        <v>15990</v>
+        <v>4967</v>
       </c>
       <c r="M22" s="76">
-        <v>0.14299999999999999</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="N22" s="76">
-        <f>K22*M22</f>
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="O22" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P22" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="O22" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B23) - ROW($B$9)</f>
         <v>14</v>
       </c>
-      <c r="C23" s="89" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="89" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="88" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="88" t="s">
-        <v>118</v>
+      <c r="C23" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="92" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="92" t="s">
+        <v>172</v>
       </c>
       <c r="H23" s="31">
-        <v>1</v>
-      </c>
-      <c r="I23" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J23" s="89" t="s">
-        <v>140</v>
+        <v>3</v>
+      </c>
+      <c r="I23" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J23" s="93" t="s">
+        <v>217</v>
       </c>
       <c r="K23" s="38">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L23" s="38">
-        <v>10565</v>
+        <v>202531</v>
       </c>
       <c r="M23" s="77">
-        <v>0.58599999999999997</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="N23" s="77">
-        <f>K23*M23</f>
-        <v>2.3439999999999999</v>
-      </c>
-      <c r="O23" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P23" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="O23" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
       <c r="B24" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B24) - ROW($B$9)</f>
         <v>15</v>
       </c>
-      <c r="C24" s="87" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="87" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="90" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="90" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="90" t="s">
-        <v>119</v>
+      <c r="C24" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="94" t="s">
+        <v>144</v>
+      </c>
+      <c r="G24" s="94" t="s">
+        <v>173</v>
       </c>
       <c r="H24" s="29">
         <v>1</v>
       </c>
-      <c r="I24" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J24" s="93" t="s">
-        <v>141</v>
+      <c r="I24" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24" s="97" t="s">
+        <v>218</v>
       </c>
       <c r="K24" s="37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L24" s="37">
-        <v>17046</v>
+        <v>17118</v>
       </c>
       <c r="M24" s="76">
-        <v>1</v>
+        <v>1.6299999999999999E-2</v>
       </c>
       <c r="N24" s="76">
-        <v>4</v>
-      </c>
-      <c r="O24" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P24" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="O24" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="52"/>
       <c r="B25" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B25) - ROW($B$9)</f>
         <v>16</v>
       </c>
-      <c r="C25" s="89" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="E25" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="88" t="s">
-        <v>120</v>
+      <c r="C25" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="92" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="92" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="92" t="s">
+        <v>174</v>
       </c>
       <c r="H25" s="31">
-        <v>1</v>
-      </c>
-      <c r="I25" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J25" s="89" t="s">
-        <v>142</v>
+        <v>4</v>
+      </c>
+      <c r="I25" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25" s="93" t="s">
+        <v>219</v>
       </c>
       <c r="K25" s="38">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L25" s="38">
-        <v>3230</v>
+        <v>7375</v>
       </c>
       <c r="M25" s="77">
-        <v>0.28299999999999997</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="N25" s="77">
-        <f>K25*M25</f>
-        <v>1.4149999999999998</v>
-      </c>
-      <c r="O25" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P25" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2.84</v>
+      </c>
+      <c r="O25" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52"/>
       <c r="B26" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B26) - ROW($B$9)</f>
         <v>17</v>
       </c>
-      <c r="C26" s="87" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="87" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="90" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="90" t="s">
-        <v>121</v>
+      <c r="C26" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="94" t="s">
+        <v>175</v>
       </c>
       <c r="H26" s="29">
-        <v>1</v>
-      </c>
-      <c r="I26" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J26" s="93" t="s">
-        <v>143</v>
+        <v>7</v>
+      </c>
+      <c r="I26" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J26" s="97" t="s">
+        <v>220</v>
       </c>
       <c r="K26" s="37">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="L26" s="37">
-        <v>321</v>
+        <v>8369</v>
       </c>
       <c r="M26" s="76">
-        <v>2.63</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="N26" s="76">
-        <f>K26*M26</f>
-        <v>10.52</v>
-      </c>
-      <c r="O26" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P26" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.18759999999999999</v>
+      </c>
+      <c r="O26" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="52"/>
       <c r="B27" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B27) - ROW($B$9)</f>
         <v>18</v>
       </c>
-      <c r="C27" s="89" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="89" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="88" t="s">
-        <v>100</v>
-      </c>
-      <c r="G27" s="88" t="s">
-        <v>122</v>
+      <c r="C27" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" s="92" t="s">
+        <v>176</v>
       </c>
       <c r="H27" s="31">
-        <v>2</v>
-      </c>
-      <c r="I27" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J27" s="89" t="s">
-        <v>144</v>
+        <v>5</v>
+      </c>
+      <c r="I27" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J27" s="93" t="s">
+        <v>221</v>
       </c>
       <c r="K27" s="38">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L27" s="38">
-        <v>39066</v>
+        <v>6564</v>
       </c>
       <c r="M27" s="77">
-        <v>0.63800000000000001</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="N27" s="77">
-        <f>K27*M27</f>
-        <v>6.38</v>
-      </c>
-      <c r="O27" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P27" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="O27" s="102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52"/>
       <c r="B28" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B28) - ROW($B$9)</f>
         <v>19</v>
       </c>
-      <c r="C28" s="87" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="90" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="90" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="90" t="s">
-        <v>123</v>
+      <c r="C28" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="F28" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="94" t="s">
+        <v>177</v>
       </c>
       <c r="H28" s="29">
-        <v>1</v>
-      </c>
-      <c r="I28" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="J28" s="93" t="s">
-        <v>145</v>
+        <v>2</v>
+      </c>
+      <c r="I28" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J28" s="97" t="s">
+        <v>222</v>
       </c>
       <c r="K28" s="37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L28" s="37">
-        <v>1430</v>
+        <v>58910</v>
       </c>
       <c r="M28" s="76">
-        <v>0.65500000000000003</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="N28" s="76">
-        <f>K28*M28</f>
-        <v>3.2750000000000004</v>
-      </c>
-      <c r="O28" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P28" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.08</v>
+      </c>
+      <c r="O28" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="52"/>
       <c r="B29" s="30">
-        <f t="shared" si="0"/>
+        <f>ROW(B29) - ROW($B$9)</f>
         <v>20</v>
       </c>
-      <c r="C29" s="89" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="89" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="88" t="s">
+      <c r="C29" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="88" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29" s="88" t="s">
-        <v>124</v>
+      <c r="E29" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="F29" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="92" t="s">
+        <v>178</v>
       </c>
       <c r="H29" s="31">
-        <v>1</v>
-      </c>
-      <c r="I29" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="J29" s="89" t="s">
-        <v>146</v>
+        <v>4</v>
+      </c>
+      <c r="I29" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J29" s="93" t="s">
+        <v>223</v>
       </c>
       <c r="K29" s="38">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L29" s="38">
-        <v>222</v>
+        <v>745</v>
       </c>
       <c r="M29" s="77">
-        <v>0.31900000000000001</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="N29" s="77">
-        <f>K29*M29</f>
-        <v>3.19</v>
-      </c>
-      <c r="O29" s="98" t="s">
-        <v>152</v>
-      </c>
-      <c r="P29" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="O29" s="102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="28">
-        <f t="shared" si="0"/>
+        <f>ROW(B30) - ROW($B$9)</f>
         <v>21</v>
       </c>
-      <c r="C30" s="108" t="s">
-        <v>163</v>
-      </c>
-      <c r="D30" s="109" t="s">
-        <v>162</v>
-      </c>
-      <c r="E30" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="90" t="s">
-        <v>125</v>
+      <c r="C30" s="91" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="94" t="s">
+        <v>179</v>
       </c>
       <c r="H30" s="29">
         <v>1</v>
       </c>
-      <c r="I30" s="91" t="s">
+      <c r="I30" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J30" s="97" t="s">
+        <v>224</v>
+      </c>
+      <c r="K30" s="37">
+        <v>10</v>
+      </c>
+      <c r="L30" s="37">
+        <v>8340</v>
+      </c>
+      <c r="M30" s="76">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="N30" s="76">
+        <v>0.09</v>
+      </c>
+      <c r="O30" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="30">
+        <f>ROW(B31) - ROW($B$9)</f>
+        <v>22</v>
+      </c>
+      <c r="C31" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="92" t="s">
+        <v>180</v>
+      </c>
+      <c r="H31" s="31">
+        <v>1</v>
+      </c>
+      <c r="I31" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J31" s="93" t="s">
+        <v>225</v>
+      </c>
+      <c r="K31" s="38">
+        <v>10</v>
+      </c>
+      <c r="L31" s="38">
+        <v>1280</v>
+      </c>
+      <c r="M31" s="77">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N31" s="77">
+        <v>0.03</v>
+      </c>
+      <c r="O31" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="52"/>
+      <c r="B32" s="28">
+        <f>ROW(B32) - ROW($B$9)</f>
+        <v>23</v>
+      </c>
+      <c r="C32" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="94" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32" s="29">
+        <v>1</v>
+      </c>
+      <c r="I32" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J32" s="97" t="s">
+        <v>226</v>
+      </c>
+      <c r="K32" s="37">
+        <v>10</v>
+      </c>
+      <c r="L32" s="37">
+        <v>102020</v>
+      </c>
+      <c r="M32" s="76">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="N32" s="76">
+        <v>3.1E-2</v>
+      </c>
+      <c r="O32" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="52"/>
+      <c r="B33" s="30">
+        <f>ROW(B33) - ROW($B$9)</f>
+        <v>24</v>
+      </c>
+      <c r="C33" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" s="92" t="s">
+        <v>182</v>
+      </c>
+      <c r="H33" s="31">
+        <v>1</v>
+      </c>
+      <c r="I33" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J33" s="93" t="s">
+        <v>227</v>
+      </c>
+      <c r="K33" s="38">
+        <v>10</v>
+      </c>
+      <c r="L33" s="38">
+        <v>91916</v>
+      </c>
+      <c r="M33" s="77">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N33" s="77">
+        <v>0.03</v>
+      </c>
+      <c r="O33" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="52"/>
+      <c r="B34" s="28">
+        <f>ROW(B34) - ROW($B$9)</f>
+        <v>25</v>
+      </c>
+      <c r="C34" s="91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="94" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="94" t="s">
+        <v>183</v>
+      </c>
+      <c r="H34" s="29">
+        <v>1</v>
+      </c>
+      <c r="I34" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J34" s="97" t="s">
+        <v>228</v>
+      </c>
+      <c r="K34" s="37">
+        <v>10</v>
+      </c>
+      <c r="L34" s="37">
+        <v>62070</v>
+      </c>
+      <c r="M34" s="76">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="N34" s="76">
+        <v>3.1E-2</v>
+      </c>
+      <c r="O34" s="101" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="52"/>
+      <c r="B35" s="30">
+        <f>ROW(B35) - ROW($B$9)</f>
+        <v>26</v>
+      </c>
+      <c r="C35" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="93" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="92" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="92" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="92" t="s">
+        <v>184</v>
+      </c>
+      <c r="H35" s="31">
+        <v>1</v>
+      </c>
+      <c r="I35" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J35" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="77"/>
+      <c r="N35" s="77"/>
+      <c r="O35" s="102" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="52"/>
+      <c r="B36" s="28">
+        <f>ROW(B36) - ROW($B$9)</f>
+        <v>27</v>
+      </c>
+      <c r="C36" s="91" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="91" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="94" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="94" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="29">
+        <v>1</v>
+      </c>
+      <c r="I36" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J36" s="97" t="s">
+        <v>230</v>
+      </c>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="76"/>
+      <c r="O36" s="101" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="52"/>
+      <c r="B37" s="30">
+        <f>ROW(B37) - ROW($B$9)</f>
+        <v>28</v>
+      </c>
+      <c r="C37" s="93" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37" s="92" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="92" t="s">
+        <v>147</v>
+      </c>
+      <c r="G37" s="92" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="31">
+        <v>1</v>
+      </c>
+      <c r="I37" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J37" s="93" t="s">
+        <v>231</v>
+      </c>
+      <c r="K37" s="38">
+        <v>4</v>
+      </c>
+      <c r="L37" s="38">
+        <v>10565</v>
+      </c>
+      <c r="M37" s="77">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="N37" s="77">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="O37" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="52"/>
+      <c r="B38" s="28">
+        <f>ROW(B38) - ROW($B$9)</f>
+        <v>29</v>
+      </c>
+      <c r="C38" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="91" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="94" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="94" t="s">
+        <v>148</v>
+      </c>
+      <c r="G38" s="94" t="s">
+        <v>187</v>
+      </c>
+      <c r="H38" s="29">
+        <v>1</v>
+      </c>
+      <c r="I38" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J38" s="97" t="s">
+        <v>232</v>
+      </c>
+      <c r="K38" s="37">
+        <v>4</v>
+      </c>
+      <c r="L38" s="37">
+        <v>16639</v>
+      </c>
+      <c r="M38" s="76">
+        <v>1</v>
+      </c>
+      <c r="N38" s="76">
+        <v>4</v>
+      </c>
+      <c r="O38" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="52"/>
+      <c r="B39" s="30">
+        <f>ROW(B39) - ROW($B$9)</f>
+        <v>30</v>
+      </c>
+      <c r="C39" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="92" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" s="92" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="92" t="s">
+        <v>188</v>
+      </c>
+      <c r="H39" s="31">
+        <v>1</v>
+      </c>
+      <c r="I39" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J39" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="K39" s="38">
+        <v>5</v>
+      </c>
+      <c r="L39" s="38">
+        <v>6844</v>
+      </c>
+      <c r="M39" s="77">
+        <v>0.22</v>
+      </c>
+      <c r="N39" s="77">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O39" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="52"/>
+      <c r="B40" s="28">
+        <f>ROW(B40) - ROW($B$9)</f>
+        <v>31</v>
+      </c>
+      <c r="C40" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="91" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="G40" s="94" t="s">
+        <v>189</v>
+      </c>
+      <c r="H40" s="29">
+        <v>1</v>
+      </c>
+      <c r="I40" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J40" s="97" t="s">
+        <v>234</v>
+      </c>
+      <c r="K40" s="37">
+        <v>4</v>
+      </c>
+      <c r="L40" s="37">
+        <v>316</v>
+      </c>
+      <c r="M40" s="76">
+        <v>2.63</v>
+      </c>
+      <c r="N40" s="76">
+        <v>10.52</v>
+      </c>
+      <c r="O40" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="52"/>
+      <c r="B41" s="30">
+        <f>ROW(B41) - ROW($B$9)</f>
+        <v>32</v>
+      </c>
+      <c r="C41" s="93" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="93" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="92" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="92" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="H41" s="31">
+        <v>2</v>
+      </c>
+      <c r="I41" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="K41" s="38">
+        <v>10</v>
+      </c>
+      <c r="L41" s="38">
+        <v>37595</v>
+      </c>
+      <c r="M41" s="77">
+        <v>0.49</v>
+      </c>
+      <c r="N41" s="77">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="O41" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="52"/>
+      <c r="B42" s="28">
+        <f>ROW(B42) - ROW($B$9)</f>
+        <v>33</v>
+      </c>
+      <c r="C42" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" s="94" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="94" t="s">
+        <v>191</v>
+      </c>
+      <c r="H42" s="29">
+        <v>1</v>
+      </c>
+      <c r="I42" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J42" s="97" t="s">
+        <v>236</v>
+      </c>
+      <c r="K42" s="37">
+        <v>5</v>
+      </c>
+      <c r="L42" s="37">
+        <v>3100</v>
+      </c>
+      <c r="M42" s="76">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="N42" s="76">
+        <v>3.2749999999999999</v>
+      </c>
+      <c r="O42" s="101" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="52"/>
+      <c r="B43" s="30">
+        <f>ROW(B43) - ROW($B$9)</f>
+        <v>34</v>
+      </c>
+      <c r="C43" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="92" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="92" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" s="92" t="s">
+        <v>192</v>
+      </c>
+      <c r="H43" s="31">
+        <v>1</v>
+      </c>
+      <c r="I43" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J43" s="93" t="s">
+        <v>237</v>
+      </c>
+      <c r="K43" s="38">
+        <v>5</v>
+      </c>
+      <c r="L43" s="38">
+        <v>0</v>
+      </c>
+      <c r="M43" s="77">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="N43" s="77">
+        <v>1.425</v>
+      </c>
+      <c r="O43" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="28">
+        <f>ROW(B44) - ROW($B$9)</f>
+        <v>35</v>
+      </c>
+      <c r="C44" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="J30" s="110">
-        <v>2288747</v>
-      </c>
-      <c r="K30" s="37">
-        <v>4</v>
-      </c>
-      <c r="L30" s="37">
-        <v>2502</v>
-      </c>
-      <c r="M30" s="76">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="N30" s="76">
-        <f>K30*M30</f>
-        <v>1.9</v>
-      </c>
-      <c r="O30" s="97" t="s">
-        <v>152</v>
-      </c>
-      <c r="P30" s="106" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="43">
-        <f>SUM(H10:H30)</f>
-        <v>27</v>
-      </c>
-      <c r="I31" s="70"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="43">
-        <f>SUM(K10:K30)</f>
-        <v>141</v>
-      </c>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42">
-        <f>SUM(N10:N30)</f>
-        <v>81.373999999999995</v>
-      </c>
-      <c r="O31" s="63"/>
-    </row>
-    <row r="32" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="102" t="s">
+      <c r="F44" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" s="94" t="s">
+        <v>193</v>
+      </c>
+      <c r="H44" s="29">
+        <v>3</v>
+      </c>
+      <c r="I44" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J44" s="97" t="s">
+        <v>238</v>
+      </c>
+      <c r="K44" s="37"/>
+      <c r="L44" s="37">
+        <v>11495</v>
+      </c>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="101" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="52"/>
+      <c r="B45" s="30">
+        <f>ROW(B45) - ROW($B$9)</f>
+        <v>36</v>
+      </c>
+      <c r="C45" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="93" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="92" t="s">
+        <v>129</v>
+      </c>
+      <c r="F45" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="G45" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="H45" s="31">
+        <v>6</v>
+      </c>
+      <c r="I45" s="96" t="s">
+        <v>201</v>
+      </c>
+      <c r="J45" s="93" t="s">
+        <v>239</v>
+      </c>
+      <c r="K45" s="38">
+        <v>24</v>
+      </c>
+      <c r="L45" s="38">
+        <v>9770</v>
+      </c>
+      <c r="M45" s="77">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="N45" s="77">
+        <v>0.35520000000000002</v>
+      </c>
+      <c r="O45" s="102" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="52"/>
+      <c r="B46" s="28">
+        <f>ROW(B46) - ROW($B$9)</f>
+        <v>37</v>
+      </c>
+      <c r="C46" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E46" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="94" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" s="94" t="s">
+        <v>195</v>
+      </c>
+      <c r="H46" s="29">
+        <v>1</v>
+      </c>
+      <c r="I46" s="95" t="s">
+        <v>201</v>
+      </c>
+      <c r="J46" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="76"/>
+      <c r="N46" s="76"/>
+      <c r="O46" s="101" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="52"/>
+      <c r="B47" s="30">
+        <f>ROW(B47) - ROW($B$9)</f>
+        <v>38</v>
+      </c>
+      <c r="C47" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="92" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" s="92" t="s">
+        <v>155</v>
+      </c>
+      <c r="G47" s="92" t="s">
+        <v>196</v>
+      </c>
+      <c r="H47" s="31">
+        <v>1</v>
+      </c>
+      <c r="I47" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="J47" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="77"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="102" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="52"/>
+      <c r="B48" s="28">
+        <f>ROW(B48) - ROW($B$9)</f>
+        <v>39</v>
+      </c>
+      <c r="C48" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="94" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" s="94" t="s">
+        <v>156</v>
+      </c>
+      <c r="G48" s="94" t="s">
+        <v>197</v>
+      </c>
+      <c r="H48" s="29">
+        <v>1</v>
+      </c>
+      <c r="I48" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="J48" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="101" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="52"/>
+      <c r="B49" s="30">
+        <f>ROW(B49) - ROW($B$9)</f>
+        <v>40</v>
+      </c>
+      <c r="C49" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="92" t="s">
+        <v>133</v>
+      </c>
+      <c r="F49" s="92" t="s">
+        <v>157</v>
+      </c>
+      <c r="G49" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="H49" s="31">
+        <v>1</v>
+      </c>
+      <c r="I49" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="J49" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="77"/>
+      <c r="N49" s="77"/>
+      <c r="O49" s="102" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="52"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="43">
+        <f>SUM(H10:H49)</f>
+        <v>75</v>
+      </c>
+      <c r="I50" s="70"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="43">
+        <f>SUM(K10:K49)</f>
+        <v>301</v>
+      </c>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42">
+        <f>SUM(N10:N49)</f>
+        <v>72.160499999999999</v>
+      </c>
+      <c r="O50" s="63"/>
+    </row>
+    <row r="51" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="52"/>
+      <c r="B51" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="102"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="46" t="s">
+      <c r="C51" s="78"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="62"/>
-    </row>
-    <row r="33" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="75" t="s">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="36"/>
+      <c r="O51" s="62"/>
+    </row>
+    <row r="52" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="52"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="83" t="s">
+      <c r="G52" s="5"/>
+      <c r="H52" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="I33" s="75"/>
-      <c r="J33" s="41" t="s">
+      <c r="I52" s="75"/>
+      <c r="J52" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="36"/>
-      <c r="L33" s="103">
-        <f>N31</f>
-        <v>81.373999999999995</v>
-      </c>
-      <c r="M33" s="104"/>
-      <c r="N33" s="84" t="s">
+      <c r="K52" s="36"/>
+      <c r="L52" s="79">
+        <f>N50</f>
+        <v>72.160499999999999</v>
+      </c>
+      <c r="M52" s="80"/>
+      <c r="N52" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="O33" s="62"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="52"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="45" t="s">
+      <c r="O52" s="62"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="52"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="72"/>
+      <c r="J53" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="105">
-        <f>L33/H33</f>
-        <v>20.343499999999999</v>
-      </c>
-      <c r="M34" s="105"/>
-      <c r="N34" s="85" t="s">
+      <c r="K53" s="6"/>
+      <c r="L53" s="81">
+        <f>L52/H52</f>
+        <v>18.040125</v>
+      </c>
+      <c r="M53" s="81"/>
+      <c r="N53" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="O34" s="62"/>
-    </row>
-    <row r="35" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="56"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
-      <c r="O35" s="64"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="O53" s="62"/>
+    </row>
+    <row r="54" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="55"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="56"/>
+      <c r="M54" s="56"/>
+      <c r="N54" s="56"/>
+      <c r="O54" s="64"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="L53:M53"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="L10:L11">
-    <cfRule type="cellIs" dxfId="43" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="79" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10:N11">
-    <cfRule type="containsBlanks" dxfId="42" priority="78">
+    <cfRule type="containsBlanks" dxfId="76" priority="78">
       <formula>LEN(TRIM(N10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="cellIs" dxfId="41" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="containsBlanks" dxfId="40" priority="73">
+    <cfRule type="containsBlanks" dxfId="74" priority="75">
       <formula>LEN(TRIM(N12))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="39" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="74" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="containsBlanks" dxfId="38" priority="71">
+    <cfRule type="containsBlanks" dxfId="72" priority="73">
       <formula>LEN(TRIM(N13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="37" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="containsBlanks" dxfId="36" priority="69">
+    <cfRule type="containsBlanks" dxfId="70" priority="71">
       <formula>LEN(TRIM(N14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="cellIs" dxfId="35" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="containsBlanks" dxfId="34" priority="65">
+    <cfRule type="containsBlanks" dxfId="68" priority="69">
       <formula>LEN(TRIM(N15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="cellIs" dxfId="33" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="68" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="containsBlanks" dxfId="32" priority="63">
+    <cfRule type="containsBlanks" dxfId="66" priority="67">
       <formula>LEN(TRIM(N16))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="31" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="66" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N17">
-    <cfRule type="containsBlanks" dxfId="30" priority="61">
+    <cfRule type="containsBlanks" dxfId="64" priority="65">
       <formula>LEN(TRIM(N17))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="27" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18">
-    <cfRule type="containsBlanks" dxfId="26" priority="57">
+    <cfRule type="containsBlanks" dxfId="62" priority="63">
       <formula>LEN(TRIM(N18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="cellIs" dxfId="25" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N19">
-    <cfRule type="containsBlanks" dxfId="24" priority="53">
+    <cfRule type="containsBlanks" dxfId="60" priority="61">
       <formula>LEN(TRIM(N19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="23" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20">
-    <cfRule type="containsBlanks" dxfId="22" priority="51">
+    <cfRule type="containsBlanks" dxfId="58" priority="59">
       <formula>LEN(TRIM(N20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21">
-    <cfRule type="containsBlanks" dxfId="20" priority="29">
+    <cfRule type="containsBlanks" dxfId="56" priority="57">
       <formula>LEN(TRIM(N21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="containsBlanks" dxfId="18" priority="27">
+    <cfRule type="containsBlanks" dxfId="54" priority="55">
       <formula>LEN(TRIM(N22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="containsBlanks" dxfId="16" priority="25">
+    <cfRule type="containsBlanks" dxfId="52" priority="53">
       <formula>LEN(TRIM(N23))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24">
-    <cfRule type="containsBlanks" dxfId="14" priority="23">
+    <cfRule type="containsBlanks" dxfId="50" priority="51">
       <formula>LEN(TRIM(N24))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25">
-    <cfRule type="containsBlanks" dxfId="12" priority="21">
+    <cfRule type="containsBlanks" dxfId="48" priority="49">
       <formula>LEN(TRIM(N25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="containsBlanks" dxfId="10" priority="19">
+    <cfRule type="containsBlanks" dxfId="46" priority="47">
       <formula>LEN(TRIM(N26))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="containsBlanks" dxfId="8" priority="17">
+    <cfRule type="containsBlanks" dxfId="44" priority="45">
       <formula>LEN(TRIM(N27))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N28">
-    <cfRule type="containsBlanks" dxfId="6" priority="15">
+    <cfRule type="containsBlanks" dxfId="42" priority="43">
       <formula>LEN(TRIM(N28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L29">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29">
-    <cfRule type="containsBlanks" dxfId="4" priority="13">
+    <cfRule type="containsBlanks" dxfId="40" priority="41">
       <formula>LEN(TRIM(N29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30">
-    <cfRule type="containsBlanks" dxfId="0" priority="7">
+    <cfRule type="containsBlanks" dxfId="38" priority="39">
       <formula>LEN(TRIM(N30))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L31">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N31">
+    <cfRule type="containsBlanks" dxfId="36" priority="37">
+      <formula>LEN(TRIM(N31))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N32">
+    <cfRule type="containsBlanks" dxfId="34" priority="35">
+      <formula>LEN(TRIM(N32))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
+    <cfRule type="containsBlanks" dxfId="32" priority="33">
+      <formula>LEN(TRIM(N33))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L34">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N34">
+    <cfRule type="containsBlanks" dxfId="30" priority="31">
+      <formula>LEN(TRIM(N34))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L35">
+    <cfRule type="cellIs" dxfId="29" priority="30" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N35">
+    <cfRule type="containsBlanks" dxfId="28" priority="29">
+      <formula>LEN(TRIM(N35))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L36">
+    <cfRule type="cellIs" dxfId="27" priority="28" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N36">
+    <cfRule type="containsBlanks" dxfId="26" priority="27">
+      <formula>LEN(TRIM(N36))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L37">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N37">
+    <cfRule type="containsBlanks" dxfId="24" priority="25">
+      <formula>LEN(TRIM(N37))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L38">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N38">
+    <cfRule type="containsBlanks" dxfId="22" priority="23">
+      <formula>LEN(TRIM(N38))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L39">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N39">
+    <cfRule type="containsBlanks" dxfId="20" priority="21">
+      <formula>LEN(TRIM(N39))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L40">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N40">
+    <cfRule type="containsBlanks" dxfId="18" priority="19">
+      <formula>LEN(TRIM(N40))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L41">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N41">
+    <cfRule type="containsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(N41))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L42">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N42">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(N42))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L43">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N43">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(N43))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L44">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N44">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(N44))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L45">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N45">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(N45))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N46">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(N46))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L47">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N47">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(N47))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L48">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N48">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(N48))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N49">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(N49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K7" r:id="rId1"/>
-    <hyperlink ref="C11" r:id="rId2" tooltip="Manufacturer" display="'RS1JE361T"/>
-    <hyperlink ref="C12" r:id="rId3" tooltip="Manufacturer" display="'BQ24296RGET"/>
-    <hyperlink ref="C13" r:id="rId4" tooltip="Manufacturer" display="'TPS630701RNMT"/>
-    <hyperlink ref="C14" r:id="rId5" tooltip="Manufacturer" display="'TPS62740DSSR"/>
-    <hyperlink ref="C16" r:id="rId6" tooltip="Manufacturer" display="'FDSD0420-H-1R5M=P3"/>
-    <hyperlink ref="C17" r:id="rId7" tooltip="Manufacturer" display="'GRM188R61C475KAAJD"/>
-    <hyperlink ref="C18" r:id="rId8" tooltip="Manufacturer" display="'MCWR06X2493FTL"/>
-    <hyperlink ref="C19" r:id="rId9" tooltip="Manufacturer" display="'MC0603B473K500CT"/>
-    <hyperlink ref="C20" r:id="rId10" tooltip="Manufacturer" display="'MC0805X226M6R3CT"/>
-    <hyperlink ref="C23" r:id="rId11" tooltip="Manufacturer" display="'MINISMDC150F/24-2"/>
-    <hyperlink ref="C24" r:id="rId12" tooltip="Manufacturer" display="'1066"/>
-    <hyperlink ref="C25" r:id="rId13" tooltip="Manufacturer" display="'LFXTAL009678"/>
-    <hyperlink ref="C26" r:id="rId14" tooltip="Manufacturer" display="'ISL1208IU8Z-T7A"/>
-    <hyperlink ref="C27" r:id="rId15" tooltip="Manufacturer" display="'U.FL-R-SMT-1(10)"/>
-    <hyperlink ref="C28" r:id="rId16" tooltip="Manufacturer" display="'BZT52C6V2"/>
-    <hyperlink ref="C29" r:id="rId17" tooltip="Manufacturer" display="'DMG6602SVT"/>
-    <hyperlink ref="D10" r:id="rId18" tooltip="Component" display="'Vishay Semiconductors"/>
-    <hyperlink ref="D11" r:id="rId19" tooltip="Component" display="'Vishay Intertechnology"/>
-    <hyperlink ref="D12" r:id="rId20" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="D13" r:id="rId21" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="D14" r:id="rId22" tooltip="Component" display="'Texas Instruments"/>
-    <hyperlink ref="D15" r:id="rId23" tooltip="Component" display="'Nexperia"/>
-    <hyperlink ref="D16" r:id="rId24" tooltip="Component" display="'Murata"/>
-    <hyperlink ref="D17" r:id="rId25" tooltip="Component" display="'Murata"/>
-    <hyperlink ref="D18" r:id="rId26" tooltip="Component" display="'Multicomp"/>
-    <hyperlink ref="D19" r:id="rId27" tooltip="Component" display="'Multicomp"/>
-    <hyperlink ref="D20" r:id="rId28" tooltip="Component" display="'Multicomp"/>
-    <hyperlink ref="D23" r:id="rId29" tooltip="Component" display="'Littelfuse"/>
-    <hyperlink ref="D24" r:id="rId30" tooltip="Component" display="'Keystone Electronics"/>
-    <hyperlink ref="D25" r:id="rId31" tooltip="Component" display="'IQD"/>
-    <hyperlink ref="D26" r:id="rId32" tooltip="Component" display="'Intersil"/>
-    <hyperlink ref="D27" r:id="rId33" tooltip="Component" display="'Hirose"/>
-    <hyperlink ref="D28" r:id="rId34" tooltip="Component" display="'Diodes Zetex"/>
-    <hyperlink ref="D29" r:id="rId35" tooltip="Component" display="'Diodes"/>
-    <hyperlink ref="J11" r:id="rId36" tooltip="Supplier" display="'9550143"/>
-    <hyperlink ref="J12" r:id="rId37" tooltip="Supplier" display="'2373541"/>
-    <hyperlink ref="J13" r:id="rId38" tooltip="Supplier" display="'2643432"/>
-    <hyperlink ref="J14" r:id="rId39" tooltip="Supplier" display="'2781752"/>
-    <hyperlink ref="J16" r:id="rId40" tooltip="Supplier" display="'2530091"/>
-    <hyperlink ref="J17" r:id="rId41" tooltip="Supplier" display="'2611924"/>
-    <hyperlink ref="J18" r:id="rId42" tooltip="Supplier" display="'2447306"/>
-    <hyperlink ref="J19" r:id="rId43" tooltip="Supplier" display="'1759116"/>
-    <hyperlink ref="J20" r:id="rId44" tooltip="Supplier" display="'1759415"/>
-    <hyperlink ref="J23" r:id="rId45" tooltip="Supplier" display="'1345929"/>
-    <hyperlink ref="J24" r:id="rId46" tooltip="Supplier" display="'2293258"/>
-    <hyperlink ref="J25" r:id="rId47" tooltip="Supplier" display="'2449398"/>
-    <hyperlink ref="J26" r:id="rId48" tooltip="Supplier" display="'2543322"/>
-    <hyperlink ref="J27" r:id="rId49" tooltip="Supplier" display="'1688077"/>
-    <hyperlink ref="J28" r:id="rId50" tooltip="Supplier" display="'1902438"/>
-    <hyperlink ref="J29" r:id="rId51" tooltip="Supplier" display="'2061522"/>
-    <hyperlink ref="D30" tooltip="Component" display="'"/>
+    <hyperlink ref="C10" r:id="rId2" tooltip="Manufacturer" display="'SE30AFG-M3/6A"/>
+    <hyperlink ref="C11" r:id="rId3" tooltip="Manufacturer" display="'RS1JE361T"/>
+    <hyperlink ref="C12" r:id="rId4" tooltip="Manufacturer" display="'RCA060310R0FKEA"/>
+    <hyperlink ref="C13" r:id="rId5" tooltip="Manufacturer" display="'BQ24296RGET"/>
+    <hyperlink ref="C14" r:id="rId6" tooltip="Manufacturer" display="'TPS630701RNMT"/>
+    <hyperlink ref="C15" r:id="rId7" tooltip="Manufacturer" display="'TPS62740DSSR"/>
+    <hyperlink ref="C16" r:id="rId8" tooltip="Manufacturer" display="'109990166"/>
+    <hyperlink ref="C17" r:id="rId9" tooltip="Manufacturer" display="'MMBT3904"/>
+    <hyperlink ref="C18" r:id="rId10" tooltip="Manufacturer" display="'2N7002,215"/>
+    <hyperlink ref="C19" r:id="rId11" tooltip="Manufacturer" display="'FDSD0420-H-1R5M=P3"/>
+    <hyperlink ref="C20" r:id="rId12" tooltip="Manufacturer" display="'GRM188R61C475KAAJD"/>
+    <hyperlink ref="C21" r:id="rId13" tooltip="Manufacturer" display="'MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, MC0805X106K160CT, CGA4J1X5R1C106K125AC, CGA4J1X5R1C106K125AC"/>
+    <hyperlink ref="C22" r:id="rId14" tooltip="Manufacturer" display="'MCWR06X2493FTL"/>
+    <hyperlink ref="C23" r:id="rId15" tooltip="Manufacturer" display="'MCWR06X1000FTL"/>
+    <hyperlink ref="C24" r:id="rId16" tooltip="Manufacturer" display="'MC0603B473K500CT"/>
+    <hyperlink ref="C25" r:id="rId17" tooltip="Manufacturer" display="'MC0805X226M6R3CT"/>
+    <hyperlink ref="C26" r:id="rId18" tooltip="Manufacturer" display="'MCMR06X103JTL"/>
+    <hyperlink ref="C27" r:id="rId19" tooltip="Manufacturer" display="'MCMR06X104JTL"/>
+    <hyperlink ref="C28" r:id="rId20" tooltip="Manufacturer" display="'MCMR06X4701FTL"/>
+    <hyperlink ref="C29" r:id="rId21" tooltip="Manufacturer" display="'MCMR06X471JTL"/>
+    <hyperlink ref="C30" r:id="rId22" tooltip="Manufacturer" display="'MCMR06X5601FTL"/>
+    <hyperlink ref="C31" r:id="rId23" tooltip="Manufacturer" display="'MCWR06X1503FTL"/>
+    <hyperlink ref="C32" r:id="rId24" tooltip="Manufacturer" display="'MCWR06X2200FTL"/>
+    <hyperlink ref="C33" r:id="rId25" tooltip="Manufacturer" display="'MCWR06X3302FTL"/>
+    <hyperlink ref="C34" r:id="rId26" tooltip="Manufacturer" display="'MCWR06X3901FTL"/>
+    <hyperlink ref="C35" r:id="rId27" tooltip="Manufacturer" display="'Loading..."/>
+    <hyperlink ref="C36" r:id="rId28" tooltip="Manufacturer" display="'Loading..."/>
+    <hyperlink ref="C37" r:id="rId29" tooltip="Manufacturer" display="'MINISMDC150F/24-2"/>
+    <hyperlink ref="C38" r:id="rId30" tooltip="Manufacturer" display="'1066"/>
+    <hyperlink ref="C39" r:id="rId31" tooltip="Manufacturer" display="'LFXTAL009678"/>
+    <hyperlink ref="C40" r:id="rId32" tooltip="Manufacturer" display="'ISL1208IU8Z-T7A"/>
+    <hyperlink ref="C41" r:id="rId33" tooltip="Manufacturer" display="'U.FL-R-SMT-1(10)"/>
+    <hyperlink ref="C42" r:id="rId34" tooltip="Manufacturer" display="'BZT52C6V2"/>
+    <hyperlink ref="C43" r:id="rId35" tooltip="Manufacturer" display="'DMG6602SVT"/>
+    <hyperlink ref="C44" r:id="rId36" tooltip="Manufacturer" display="'HSMS-C190"/>
+    <hyperlink ref="C45" r:id="rId37" tooltip="Manufacturer" display="'CR0603-J/-000ELF"/>
+    <hyperlink ref="C46" tooltip="Manufacturer" display="'"/>
+    <hyperlink ref="C47" tooltip="Manufacturer" display="'"/>
+    <hyperlink ref="C48" tooltip="Manufacturer" display="'"/>
+    <hyperlink ref="C49" tooltip="Manufacturer" display="'"/>
+    <hyperlink ref="D10" r:id="rId38" tooltip="Component" display="'Vishay Semiconductors"/>
+    <hyperlink ref="D11" r:id="rId39" tooltip="Component" display="'Vishay Intertechnology"/>
+    <hyperlink ref="D12" r:id="rId40" tooltip="Component" display="'Vishay Dale"/>
+    <hyperlink ref="D13" r:id="rId41" tooltip="Component" display="'Texas Instruments"/>
+    <hyperlink ref="D14" r:id="rId42" tooltip="Component" display="'Texas Instruments"/>
+    <hyperlink ref="D15" r:id="rId43" tooltip="Component" display="'Texas Instruments"/>
+    <hyperlink ref="D16" r:id="rId44" tooltip="Component" display="'Seeed Studio"/>
+    <hyperlink ref="D17" r:id="rId45" tooltip="Component" display="'ON Semiconductor / Fairchild"/>
+    <hyperlink ref="D18" r:id="rId46" tooltip="Component" display="'Nexperia"/>
+    <hyperlink ref="D19" r:id="rId47" tooltip="Component" display="'Murata"/>
+    <hyperlink ref="D20" r:id="rId48" tooltip="Component" display="'Murata"/>
+    <hyperlink ref="D21" r:id="rId49" tooltip="Component" display="'Multicomp, Multicomp, Multicomp, Multicomp, Multicomp, TDK, TDK"/>
+    <hyperlink ref="D22" r:id="rId50" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D23" r:id="rId51" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D24" r:id="rId52" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D25" r:id="rId53" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D26" r:id="rId54" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D27" r:id="rId55" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D28" r:id="rId56" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D29" r:id="rId57" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D30" r:id="rId58" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D31" r:id="rId59" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D32" r:id="rId60" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D33" r:id="rId61" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D34" r:id="rId62" tooltip="Component" display="'Multicomp"/>
+    <hyperlink ref="D35" r:id="rId63" tooltip="Component" display="'Loading..."/>
+    <hyperlink ref="D36" r:id="rId64" tooltip="Component" display="'Loading..."/>
+    <hyperlink ref="D37" r:id="rId65" tooltip="Component" display="'Littelfuse"/>
+    <hyperlink ref="D38" r:id="rId66" tooltip="Component" display="'Keystone Electronics"/>
+    <hyperlink ref="D39" r:id="rId67" tooltip="Component" display="'IQD"/>
+    <hyperlink ref="D40" r:id="rId68" tooltip="Component" display="'Intersil"/>
+    <hyperlink ref="D41" r:id="rId69" tooltip="Component" display="'Hirose"/>
+    <hyperlink ref="D42" r:id="rId70" tooltip="Component" display="'Diodes Zetex"/>
+    <hyperlink ref="D43" r:id="rId71" tooltip="Component" display="'Diodes"/>
+    <hyperlink ref="D44" r:id="rId72" tooltip="Component" display="'Broadcom Avago"/>
+    <hyperlink ref="D45" r:id="rId73" tooltip="Component" display="'Bourns"/>
+    <hyperlink ref="D46" tooltip="Component" display="'"/>
+    <hyperlink ref="D47" tooltip="Component" display="'"/>
+    <hyperlink ref="D48" tooltip="Component" display="'"/>
+    <hyperlink ref="D49" tooltip="Component" display="'"/>
+    <hyperlink ref="J10" r:id="rId74" tooltip="Supplier" display="'2313878"/>
+    <hyperlink ref="J11" r:id="rId75" tooltip="Supplier" display="'9550143"/>
+    <hyperlink ref="J12" r:id="rId76" tooltip="Supplier" display="'2616585"/>
+    <hyperlink ref="J13" r:id="rId77" tooltip="Supplier" display="'2373541"/>
+    <hyperlink ref="J14" r:id="rId78" tooltip="Supplier" display="'2643432"/>
+    <hyperlink ref="J15" r:id="rId79" tooltip="Supplier" display="'2781752"/>
+    <hyperlink ref="J16" r:id="rId80" tooltip="Supplier" display="'1597-1488-ND"/>
+    <hyperlink ref="J17" r:id="rId81" tooltip="Supplier" display="'9846727"/>
+    <hyperlink ref="J18" r:id="rId82" tooltip="Supplier" display="'1510761"/>
+    <hyperlink ref="J19" r:id="rId83" tooltip="Supplier" display="'2530091"/>
+    <hyperlink ref="J20" r:id="rId84" tooltip="Supplier" display="'2611924"/>
+    <hyperlink ref="J21" r:id="rId85" tooltip="Supplier" display="'2320856, 2320856, 2320856, 2320856, 2320856, 2210948RL, 2210948RL"/>
+    <hyperlink ref="J22" r:id="rId86" tooltip="Supplier" display="'2447306"/>
+    <hyperlink ref="J23" r:id="rId87" tooltip="Supplier" display="'2447227"/>
+    <hyperlink ref="J24" r:id="rId88" tooltip="Supplier" display="'1759116"/>
+    <hyperlink ref="J25" r:id="rId89" tooltip="Supplier" display="'1759415"/>
+    <hyperlink ref="J26" r:id="rId90" tooltip="Supplier" display="'2073356"/>
+    <hyperlink ref="J27" r:id="rId91" tooltip="Supplier" display="'2073357"/>
+    <hyperlink ref="J28" r:id="rId92" tooltip="Supplier" display="'2073509"/>
+    <hyperlink ref="J29" r:id="rId93" tooltip="Supplier" display="'2073513"/>
+    <hyperlink ref="J30" r:id="rId94" tooltip="Supplier" display="'2073537"/>
+    <hyperlink ref="J31" r:id="rId95" tooltip="Supplier" display="'2447254"/>
+    <hyperlink ref="J32" r:id="rId96" tooltip="Supplier" display="'2447298"/>
+    <hyperlink ref="J33" r:id="rId97" tooltip="Supplier" display="'2447342"/>
+    <hyperlink ref="J34" r:id="rId98" tooltip="Supplier" display="'2447363"/>
+    <hyperlink ref="J35" r:id="rId99" tooltip="Supplier" display="'2688519"/>
+    <hyperlink ref="J36" r:id="rId100" tooltip="Supplier" display="'2463510"/>
+    <hyperlink ref="J37" r:id="rId101" tooltip="Supplier" display="'1345929"/>
+    <hyperlink ref="J38" r:id="rId102" tooltip="Supplier" display="'2293258"/>
+    <hyperlink ref="J39" r:id="rId103" tooltip="Supplier" display="'2449398"/>
+    <hyperlink ref="J40" r:id="rId104" tooltip="Supplier" display="'2543322"/>
+    <hyperlink ref="J41" r:id="rId105" tooltip="Supplier" display="'1688077"/>
+    <hyperlink ref="J42" r:id="rId106" tooltip="Supplier" display="'1902438"/>
+    <hyperlink ref="J43" r:id="rId107" tooltip="Supplier" display="'2061522"/>
+    <hyperlink ref="J44" r:id="rId108" tooltip="Supplier" display="'2497356"/>
+    <hyperlink ref="J45" r:id="rId109" tooltip="Supplier" display="'2008343"/>
+    <hyperlink ref="J46" tooltip="Supplier" display="'"/>
+    <hyperlink ref="J47" tooltip="Supplier" display="'"/>
+    <hyperlink ref="J48" tooltip="Supplier" display="'"/>
+    <hyperlink ref="J49" tooltip="Supplier" display="'"/>
   </hyperlinks>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.59055118110236227" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId52"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId110"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LCreated by FEDEVEL&amp;CMotherboard, Processor and Microcontroller Board Design&amp;Rhttp://www.fedevel.com</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId53"/>
+  <drawing r:id="rId111"/>
 </worksheet>
 </file>
 
@@ -3999,15 +5407,15 @@
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
-        <v>153</v>
+      <c r="B1" s="103" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="104" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4015,7 +5423,7 @@
       <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="105" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4023,7 +5431,7 @@
       <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="104" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4031,31 +5439,31 @@
       <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="101" t="s">
-        <v>153</v>
+      <c r="B5" s="105" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="100" t="s">
-        <v>154</v>
+      <c r="B6" s="104" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="101" t="s">
-        <v>155</v>
+      <c r="B7" s="105" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="104" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4063,7 +5471,7 @@
       <c r="A9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="105" t="s">
         <v>31</v>
       </c>
     </row>
@@ -4071,40 +5479,40 @@
       <c r="A10" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="100" t="s">
-        <v>156</v>
+      <c r="B10" s="104" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="101" t="s">
-        <v>157</v>
+      <c r="B11" s="105" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="100" t="s">
-        <v>158</v>
+      <c r="B12" s="104" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="101" t="s">
-        <v>159</v>
+      <c r="B13" s="105" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="100" t="s">
-        <v>160</v>
+      <c r="B14" s="104" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>